<commit_message>
Iniciando implementação do modelo de ML. Falta funcionar a predição
</commit_message>
<xml_diff>
--- a/client/sollytch.xlsx
+++ b/client/sollytch.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\edu\sollytch-chain\client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C91521-3F3F-4E62-8559-81F91B3F8C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>test_id</t>
   </si>
@@ -124,15 +138,6 @@
     <t>incerteza_estimativa_ppb</t>
   </si>
   <si>
-    <t>acao_recomendada</t>
-  </si>
-  <si>
-    <t>result_class</t>
-  </si>
-  <si>
-    <t>qc_status</t>
-  </si>
-  <si>
     <t>TEST-00001</t>
   </si>
   <si>
@@ -172,12 +177,6 @@
     <t>refrigerado</t>
   </si>
   <si>
-    <t>retestar_e_confirmar_amostragem</t>
-  </si>
-  <si>
-    <t>negative</t>
-  </si>
-  <si>
     <t>TEST-00009</t>
   </si>
   <si>
@@ -208,9 +207,6 @@
     <t>CAL1008</t>
   </si>
   <si>
-    <t>warn</t>
-  </si>
-  <si>
     <t>TEST-00093</t>
   </si>
   <si>
@@ -257,9 +253,6 @@
   </si>
   <si>
     <t>CAL1060</t>
-  </si>
-  <si>
-    <t>positive</t>
   </si>
   <si>
     <t>TEST-00111</t>
@@ -289,25 +282,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -317,7 +310,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -339,56 +332,60 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -578,20 +575,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,55 +705,49 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+    </row>
+    <row r="2" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="B2" s="3">
+        <v>45867.634722222218</v>
+      </c>
+      <c r="C2" s="4">
+        <v>-22.862919999999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-43.236545999999997</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3">
-        <v>45867.63472222222</v>
-      </c>
-      <c r="C2" s="4">
-        <v>-22.86292</v>
-      </c>
-      <c r="D2" s="4">
-        <v>-43.236546</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="K2" s="4">
-        <v>478.0</v>
+        <v>478</v>
       </c>
       <c r="L2" s="4">
-        <v>19.56</v>
+        <v>19.559999999999999</v>
       </c>
       <c r="M2" s="4">
-        <v>540.8</v>
+        <v>540.79999999999995</v>
       </c>
       <c r="N2" s="5" t="b">
         <v>1</v>
@@ -772,7 +768,7 @@
         <v>24.1</v>
       </c>
       <c r="T2" s="4">
-        <v>72.6</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="U2" s="4">
         <v>327.8</v>
@@ -781,13 +777,13 @@
         <v>0.3</v>
       </c>
       <c r="W2" s="4">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="X2" s="4">
         <v>80.2</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z2" s="5" t="b">
         <v>1</v>
@@ -797,16 +793,16 @@
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="AG2" s="5" t="b">
         <v>1</v>
@@ -815,7 +811,7 @@
         <v>8.82</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AJ2" s="4">
         <v>24.16</v>
@@ -823,61 +819,55 @@
       <c r="AK2" s="4">
         <v>3.15</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="6"/>
+    </row>
+    <row r="3" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45870.525694444441</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-22.861256000000001</v>
+      </c>
+      <c r="D3" s="4">
+        <v>-43.242643000000001</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AN2" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="3">
-        <v>45870.52569444444</v>
-      </c>
-      <c r="C3" s="4">
-        <v>-22.861256</v>
-      </c>
-      <c r="D3" s="4">
-        <v>-43.242643</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="K3" s="4">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="L3" s="4">
         <v>20.13</v>
       </c>
       <c r="M3" s="4">
-        <v>315.0</v>
+        <v>315</v>
       </c>
       <c r="N3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="4">
-        <v>79.6</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="P3" s="4">
         <v>6.22</v>
@@ -886,7 +876,7 @@
         <v>7.8</v>
       </c>
       <c r="R3" s="4">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="S3" s="4">
         <v>25.4</v>
@@ -904,10 +894,10 @@
         <v>24.6</v>
       </c>
       <c r="X3" s="4">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Z3" s="5" t="b">
         <v>0</v>
@@ -916,28 +906,28 @@
         <v>1</v>
       </c>
       <c r="AB3" s="4">
-        <v>0.302</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="AH3" s="4">
-        <v>8.88</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AJ3" s="4">
         <v>24.12</v>
@@ -945,49 +935,43 @@
       <c r="AK3" s="4">
         <v>4.41</v>
       </c>
-      <c r="AL3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN3" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="7"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
-        <v>45895.55416666667</v>
+        <v>45895.554166666669</v>
       </c>
       <c r="C4" s="4">
         <v>-22.974788</v>
       </c>
       <c r="D4" s="4">
-        <v>-43.23629</v>
+        <v>-43.236289999999997</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K4" s="4">
-        <v>128.0</v>
+        <v>128</v>
       </c>
       <c r="L4" s="4">
         <v>19.12</v>
@@ -1023,13 +1007,13 @@
         <v>4.7</v>
       </c>
       <c r="W4" s="4">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="X4" s="4">
         <v>127.4</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z4" s="5" t="b">
         <v>0</v>
@@ -1038,19 +1022,19 @@
         <v>1</v>
       </c>
       <c r="AB4" s="4">
-        <v>0.172</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG4" s="5" t="b">
         <v>1</v>
@@ -1059,7 +1043,7 @@
         <v>9.25</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AJ4" s="4">
         <v>22.97</v>
@@ -1067,49 +1051,43 @@
       <c r="AK4" s="4">
         <v>1.89</v>
       </c>
-      <c r="AL4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN4" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="6"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3">
-        <v>45879.78541666667</v>
+        <v>45879.785416666673</v>
       </c>
       <c r="C5" s="4">
         <v>-22.876814</v>
       </c>
       <c r="D5" s="4">
-        <v>-43.216012</v>
+        <v>-43.216011999999999</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K5" s="4">
-        <v>232.0</v>
+        <v>232</v>
       </c>
       <c r="L5" s="4">
         <v>23.52</v>
@@ -1130,28 +1108,28 @@
         <v>25.5</v>
       </c>
       <c r="R5" s="4">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="S5" s="4">
         <v>20.5</v>
       </c>
       <c r="T5" s="4">
-        <v>81.9</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="U5" s="4">
-        <v>273.1</v>
+        <v>273.10000000000002</v>
       </c>
       <c r="V5" s="4">
         <v>3.8</v>
       </c>
       <c r="W5" s="4">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="X5" s="4">
         <v>78.7</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z5" s="5" t="b">
         <v>0</v>
@@ -1163,16 +1141,16 @@
         <v>0.13</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG5" s="5" t="b">
         <v>1</v>
@@ -1181,7 +1159,7 @@
         <v>18.04</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AJ5" s="4">
         <v>30.09</v>
@@ -1189,49 +1167,43 @@
       <c r="AK5" s="4">
         <v>5.47</v>
       </c>
-      <c r="AL5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN5" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="7"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3">
         <v>45868.57708333333</v>
       </c>
       <c r="C6" s="4">
-        <v>-22.859084</v>
+        <v>-22.859083999999999</v>
       </c>
       <c r="D6" s="4">
-        <v>-43.232471</v>
+        <v>-43.232470999999997</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="K6" s="4">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="L6" s="4">
         <v>25.27</v>
@@ -1249,7 +1221,7 @@
         <v>6.57</v>
       </c>
       <c r="Q6" s="4">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="R6" s="4">
         <v>23.1</v>
@@ -1258,13 +1230,13 @@
         <v>33.9</v>
       </c>
       <c r="T6" s="4">
-        <v>66.6</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="U6" s="4">
-        <v>559.7</v>
+        <v>559.70000000000005</v>
       </c>
       <c r="V6" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="4">
         <v>28.3</v>
@@ -1273,7 +1245,7 @@
         <v>29.8</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Z6" s="5" t="b">
         <v>0</v>
@@ -1283,16 +1255,16 @@
       </c>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG6" s="5" t="b">
         <v>1</v>
@@ -1301,25 +1273,19 @@
         <v>8.94</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AJ6" s="4">
-        <v>32.48</v>
+        <v>32.479999999999997</v>
       </c>
       <c r="AK6" s="4">
         <v>3.03</v>
       </c>
-      <c r="AL6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN6" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>